<commit_message>
Asset Patch - work enabling Outstation Patcher to work with different floc levels (output for Phase 1 implemented).
</commit_message>
<xml_diff>
--- a/fsharp/asset-patch/outstation-patcher/excel-sample/WorkListSample.xlsx
+++ b/fsharp/asset-patch/outstation-patcher/excel-sample/WorkListSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-trafo\fsharp\asset-patch\outstation-patcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474A6659-6CA1-4DC6-83E7-A917BBCEBACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3725F06-31D9-4EA9-84C6-15E54E198322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>BRI01</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Telemetry System</t>
+  </si>
+  <si>
+    <t>System Code</t>
+  </si>
+  <si>
+    <t>SYS01</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA0B99-BC0C-4E9D-804B-8BEC68776EFA}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,17 +464,17 @@
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -488,22 +494,25 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -523,18 +532,21 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Asset Patch - work fleshing out the Outstation Patcher.
</commit_message>
<xml_diff>
--- a/fsharp/asset-patch/outstation-patcher/excel-sample/WorkListSample.xlsx
+++ b/fsharp/asset-patch/outstation-patcher/excel-sample/WorkListSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-trafo\fsharp\asset-patch\outstation-patcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3725F06-31D9-4EA9-84C6-15E54E198322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0703E8FB-41B6-4B40-80F8-38A9FE424619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA0B99-BC0C-4E9D-804B-8BEC68776EFA}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>